<commit_message>
finish a raw version
</commit_message>
<xml_diff>
--- a/统计数据.xlsx
+++ b/统计数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PKU\20fall\可视化\Visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PKU\可视化\hw2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9C440A-DC45-49EE-9C9E-18E86BBDFB36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF17CFD-7D2E-45AF-9D44-B58F5085C1CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>女性升高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>男性寿命</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,6 +191,10 @@
   </si>
   <si>
     <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女性身高</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -523,12 +523,12 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,27 +536,27 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2">
         <v>179.9</v>
@@ -571,18 +571,18 @@
         <v>83.02</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>177.3</v>
@@ -597,18 +597,18 @@
         <v>81.14</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>178.3</v>
@@ -623,18 +623,18 @@
         <v>83.06</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>175.7</v>
@@ -649,18 +649,18 @@
         <v>77.02</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>165.4</v>
@@ -675,18 +675,18 @@
         <v>73.05</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>172.7</v>
@@ -701,18 +701,18 @@
         <v>76.22</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>166.7</v>
@@ -727,18 +727,18 @@
         <v>59.11</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>173</v>
@@ -753,18 +753,18 @@
         <v>78.12</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>173.7</v>
@@ -779,18 +779,18 @@
         <v>84.63</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>172.5</v>
@@ -805,18 +805,18 @@
         <v>77.86</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>164.9</v>
@@ -831,18 +831,18 @@
         <v>68.930000000000007</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>176.5</v>
@@ -857,18 +857,18 @@
         <v>83.78</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>170.7</v>
@@ -883,18 +883,18 @@
         <v>86.58</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>177.5</v>
@@ -909,18 +909,18 @@
         <v>82.39</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>171.6</v>
@@ -935,18 +935,18 @@
         <v>79.83</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>175</v>
@@ -961,18 +961,18 @@
         <v>85.05</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>171.5</v>
@@ -987,18 +987,18 @@
         <v>83.5</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>177.1</v>
@@ -1013,18 +1013,18 @@
         <v>81.25</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>169.1</v>
@@ -1039,18 +1039,18 @@
         <v>73.290000000000006</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>175.6</v>
@@ -1065,18 +1065,18 @@
         <v>86.49</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>177.4</v>
@@ -1091,18 +1091,18 @@
         <v>83.59</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>178</v>
@@ -1117,18 +1117,18 @@
         <v>84.28</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>160.80000000000001</v>
@@ -1143,18 +1143,18 @@
         <v>69.55</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>167.9</v>
@@ -1169,18 +1169,18 @@
         <v>76.88</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>166.6</v>
@@ -1195,18 +1195,18 @@
         <v>75.47</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>169</v>
@@ -1221,18 +1221,18 @@
         <v>78.930000000000007</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>178.4</v>
@@ -1247,18 +1247,18 @@
         <v>85.23</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>170.4</v>
@@ -1273,18 +1273,18 @@
         <v>84.12</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>172</v>
@@ -1299,18 +1299,18 @@
         <v>73.27</v>
       </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>178.2</v>
@@ -1325,18 +1325,18 @@
         <v>83.71</v>
       </c>
       <c r="F31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>182.5</v>
@@ -1351,18 +1351,18 @@
         <v>83.14</v>
       </c>
       <c r="F32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>167.8</v>
@@ -1377,18 +1377,18 @@
         <v>77.58</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>161.19999999999999</v>
@@ -1403,13 +1403,13 @@
         <v>71.55</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>